<commit_message>
fix Sum bugs in Ai model
</commit_message>
<xml_diff>
--- a/FoodDelivery.Services/Ai/segmentation_results.xlsx
+++ b/FoodDelivery.Services/Ai/segmentation_results.xlsx
@@ -477,21 +477,21 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>330</v>
       </c>
       <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>New Customer</t>
+          <t>High Value</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>660</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -502,87 +502,87 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Admin@Food.com</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>New Customer</t>
+          <t>High Value</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>5760</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>High Risk</t>
+          <t>Low Risk</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>eng.ahmedyaseen4</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>High Value</t>
+          <t>Low Value</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3600</v>
+        <v>600</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Low Risk</t>
+          <t>High Risk</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>eng.ahmedyaseen4</t>
+          <t>Mohand</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>New Customer</t>
+          <t>Low Value</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Low Risk</t>
+          <t>High Risk</t>
         </is>
       </c>
     </row>
@@ -599,11 +599,11 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>New Customer</t>
+          <t>Low Value</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Low Risk</t>
+          <t>High Risk</t>
         </is>
       </c>
     </row>
@@ -622,21 +622,21 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5100</v>
+        <v>20100</v>
       </c>
       <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>New Customer</t>
+          <t>Medium Value</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5100</v>
+        <v>40200</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>

</xml_diff>